<commit_message>
Updated PRT model - 2025-07-28 19:38
</commit_message>
<xml_diff>
--- a/VerveStacks_PRT/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_PRT/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_PRT\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5B5DC6-34B8-4B04-97BD-0A43E7299BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B10AF4D-09E7-45C1-8258-C968F9D743EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,7 +682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930DD4D4-815A-4E99-A9FE-B4DAB548F7CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F76F25-31C3-4BAC-AD21-E9AEB83C4B52}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated PRT model - 2025-07-28 20:00
</commit_message>
<xml_diff>
--- a/VerveStacks_PRT/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_PRT/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_PRT\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B10AF4D-09E7-45C1-8258-C968F9D743EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CBABAB-D664-436E-8A40-B2351173C973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,7 +682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F76F25-31C3-4BAC-AD21-E9AEB83C4B52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909304DB-5F40-496C-B611-8BBAC8C2A767}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>